<commit_message>
fpga ipc uintr freq test
</commit_message>
<xml_diff>
--- a/测试/IPC性能.xlsx
+++ b/测试/IPC性能.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ctrlz/workSpace/openingreport-ldhai2023/测试/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1062B8C1-E0B3-7F4D-A265-D5D7BFA72157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5041017C-48F3-BA41-B9A4-5D1DCC4B824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="3" xr2:uid="{DA4805F4-04B1-CA43-9DDD-E0DA8EA5F629}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{DA4805F4-04B1-CA43-9DDD-E0DA8EA5F629}"/>
   </bookViews>
   <sheets>
     <sheet name="qemu_ipc" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="47">
   <si>
     <t>async-smp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6221,6 +6221,598 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>中断频率随负载变化图</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fpga_ipc!$X$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>并发 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$49:$AB$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$50:$AB$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.46779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11269999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A93B-194F-BC42-CEB6DF17D4C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fpga_ipc!$X$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>并发 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$49:$AB$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$51:$AB$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.4158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A93B-194F-BC42-CEB6DF17D4C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fpga_ipc!$X$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>并发 16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$49:$AB$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$Y$52:$AB$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.34939999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A93B-194F-BC42-CEB6DF17D4C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1396637231"/>
+        <c:axId val="972811584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1396637231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="972811584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="972811584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1396637231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>Socket</a:t>
             </a:r>
@@ -6932,7 +7524,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -7676,7 +8268,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -8416,7 +9008,757 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>用户态中断频率</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.6208729582278979E-2"/>
+          <c:y val="0.1731895416218481"/>
+          <c:w val="0.93393895555058837"/>
+          <c:h val="0.77101603530606422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qemu_ipc!$AM$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up_server</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$16:$AS$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50029999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1899999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3DEB-5C48-A80A-F4C64B20C66B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qemu_ipc!$AM$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up_client</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$17:$AS$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1899999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3DEB-5C48-A80A-F4C64B20C66B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qemu_ipc!$AM$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>smp_server</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$18:$AS$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50170000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44230000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42559999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42149999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3DEB-5C48-A80A-F4C64B20C66B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qemu_ipc!$AM$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>smp_client</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>qemu_ipc!$AN$19:$AS$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3DEB-5C48-A80A-F4C64B20C66B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="929224688"/>
+        <c:axId val="929225504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="929224688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929225504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="929225504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929224688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -9099,756 +10441,6 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>用户态中断频率</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.6208729582278979E-2"/>
-          <c:y val="0.1731895416218481"/>
-          <c:w val="0.93393895555058837"/>
-          <c:h val="0.77101603530606422"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>qemu_ipc!$AM$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up_server</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$16:$AS$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50029999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25040000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.12559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.3399999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1899999999999998E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3DEB-5C48-A80A-F4C64B20C66B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>qemu_ipc!$AM$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up_client</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$17:$AS$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50049999999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25040000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.12559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.3399999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1899999999999998E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3DEB-5C48-A80A-F4C64B20C66B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>qemu_ipc!$AM$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>smp_server</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent3">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$18:$AS$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50170000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.49690000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.44230000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42559999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.42149999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3DEB-5C48-A80A-F4C64B20C66B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>qemu_ipc!$AM$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>smp_client</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent4">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>qemu_ipc!$AN$19:$AS$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50049999999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.31040000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13189999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.10290000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1065</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3DEB-5C48-A80A-F4C64B20C66B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="929224688"/>
-        <c:axId val="929225504"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="929224688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:noFill/>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="929225504"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="929225504"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="929224688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
@@ -15656,6 +16248,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -21855,6 +22487,544 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -26710,6 +27880,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>166511</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>472723</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>143933</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="图表 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2CEF91-2178-7C4E-AAFD-9C16589D7BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -27161,8 +28367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE31C07-FDF3-8D4E-AAE0-9812488F355C}">
   <dimension ref="A2:BA42"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP12" sqref="AP12"/>
+    <sheetView topLeftCell="S21" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM38" sqref="AM38:AQ42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28467,10 +29673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6E50E1-FA69-4847-B614-76E5EFFC3D26}">
-  <dimension ref="A2:T118"/>
+  <dimension ref="A2:AB118"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="L24" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -29087,18 +30293,81 @@
         <v>6946</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:28">
       <c r="B49" s="1"/>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>1</v>
+      </c>
+      <c r="AA49">
+        <v>2</v>
+      </c>
+      <c r="AB49">
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="50" spans="1:28">
+      <c r="X50" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y50">
+        <v>0.46779999999999999</v>
+      </c>
+      <c r="Z50">
+        <v>0.25640000000000002</v>
+      </c>
+      <c r="AA50">
+        <v>0.11269999999999999</v>
+      </c>
+      <c r="AB50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
+      <c r="X51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y51">
+        <v>0.4158</v>
+      </c>
+      <c r="Z51">
+        <v>0.18029999999999999</v>
+      </c>
+      <c r="AA51">
+        <v>0</v>
+      </c>
+      <c r="AB51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
+      <c r="X52" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y52">
+        <v>0.34939999999999999</v>
+      </c>
+      <c r="Z52">
+        <v>0.12809999999999999</v>
+      </c>
+      <c r="AA52">
+        <v>0</v>
+      </c>
+      <c r="AB52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28">
       <c r="A59" t="s">
         <v>21</v>
       </c>
       <c r="M59" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:28">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -29151,7 +30420,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:28">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -29204,7 +30473,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:28">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -29257,7 +30526,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:28">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -29310,7 +30579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:28">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -29816,7 +31085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE93499-CFB8-CF46-B176-4C0F0AC04714}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>